<commit_message>
update to prompt and context doc
</commit_message>
<xml_diff>
--- a/admin/retrieval_context.xlsx
+++ b/admin/retrieval_context.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drew_wilkins/Drews_Files/Drew/Python/VSCode/ASK/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB5C86D-8E7B-FC44-9109-3E7B483F2EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21703B7-A512-864E-BB3E-1EB29EF40DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32320" yWindow="-24100" windowWidth="29040" windowHeight="22140" activeTab="1" xr2:uid="{EB31FEF1-4297-4549-87DA-13C8F980AD35}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1508">
   <si>
     <t>Certification</t>
   </si>
@@ -4560,6 +4560,9 @@
   </si>
   <si>
     <t>get qualified</t>
+  </si>
+  <si>
+    <t>Boat crew is a competency and certification in the Auxiliary Boat Crew program. It is not part of the MSM program. It is part of Surface Operations which has requirements. See  ALAUX 002/23  2023 National Workshops, ALAUX 048/22, Calendar Year (CY) 2023 Annual Currency Maintenance Requirement Tracking for Crewmember, Coxswain, PWC Operator, and Nighttime Certification, CG-BSX Policy Letter 19-02  CHANGES TO AUXILIARY INCIDENT COMMAND SYSTEM (ICS) CORE TRAINING.</t>
   </si>
 </sst>
 </file>
@@ -4672,7 +4675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4713,9 +4716,6 @@
     <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4723,10 +4723,22 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4766,22 +4778,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4797,22 +4797,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86B674F6-EEA2-7343-94E7-3A812E52CE46}" name="Table2" displayName="Table2" ref="A1:B765" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86B674F6-EEA2-7343-94E7-3A812E52CE46}" name="Table2" displayName="Table2" ref="A1:B765" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:B765" xr:uid="{86B674F6-EEA2-7343-94E7-3A812E52CE46}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{360F639C-CD96-B945-83FA-680479071711}" name="acronym" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{24DDF167-43AA-F143-A132-2D8A8EDAF8AC}" name="definition" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{360F639C-CD96-B945-83FA-680479071711}" name="acronym" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{24DDF167-43AA-F143-A132-2D8A8EDAF8AC}" name="definition" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AE42593-E06E-834D-9409-06C6BC93EA63}" name="Table1" displayName="Table1" ref="A1:B107" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AE42593-E06E-834D-9409-06C6BC93EA63}" name="Table1" displayName="Table1" ref="A1:B107" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B107" xr:uid="{8AE42593-E06E-834D-9409-06C6BC93EA63}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0B025C42-A16E-8442-B928-48B37850B8A4}" name="term" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D6B1FFC6-2990-DC4E-8615-63C5C5E64596}" name="implication" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{0B025C42-A16E-8442-B928-48B37850B8A4}" name="term" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D6B1FFC6-2990-DC4E-8615-63C5C5E64596}" name="implication" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11489,7 +11489,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11508,7 +11508,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="1" t="s">
         <v>1503</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -11516,7 +11516,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="17">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="1" t="s">
         <v>1504</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -11524,7 +11524,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="17">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="1" t="s">
         <v>1505</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -11532,7 +11532,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="17">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="1" t="s">
         <v>1506</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -11548,7 +11548,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="1" t="s">
         <v>1497</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -11596,14 +11596,14 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="17">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="1" t="s">
         <v>1496</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1495</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17">
+    <row r="14" spans="1:2" ht="34">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -11619,12 +11619,12 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17">
+    <row r="16" spans="1:2" ht="51">
       <c r="A16" s="1" t="s">
         <v>1456</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1495</v>
+        <v>1507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>